<commit_message>
Add equipment rarity progression data + tool to import
</commit_message>
<xml_diff>
--- a/ExcelData/Final-roguelike-csv-data.xlsx
+++ b/ExcelData/Final-roguelike-csv-data.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\final-roguelike\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B67B63-6247-4506-9458-88BCC08FB3B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A4D150-D638-44BA-AD00-6D96A8B81851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1AC6DEF8-C7DB-40D9-87ED-5EA8BEC70639}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1AC6DEF8-C7DB-40D9-87ED-5EA8BEC70639}"/>
   </bookViews>
   <sheets>
     <sheet name="AttributeTierProgression" sheetId="1" r:id="rId1"/>
+    <sheet name="EquipmentRarityProgression" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Level</t>
   </si>
@@ -54,6 +55,27 @@
   </si>
   <si>
     <t>Sum</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Common</t>
+  </si>
+  <si>
+    <t>Uncommon</t>
+  </si>
+  <si>
+    <t>Rare</t>
+  </si>
+  <si>
+    <t>Epic</t>
+  </si>
+  <si>
+    <t>Legendary</t>
+  </si>
+  <si>
+    <t>SUM CHECK</t>
   </si>
 </sst>
 </file>
@@ -118,7 +140,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -135,6 +157,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -472,7 +497,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63EA9316-DF04-442E-BAE7-EAA1D4EA1AC7}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D29" sqref="D29"/>
     </sheetView>
@@ -1031,4 +1056,265 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FB7F967-0E1F-423A-A242-28F419A2F4C6}">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="9.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" style="3"/>
+    <col min="6" max="6" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>75</v>
+      </c>
+      <c r="C2" s="3">
+        <v>20</v>
+      </c>
+      <c r="D2" s="3">
+        <v>5</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <f>SUM(B2:F2)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>50</v>
+      </c>
+      <c r="C3" s="3">
+        <v>40</v>
+      </c>
+      <c r="D3" s="3">
+        <v>10</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G10" si="0">SUM(B3:F3)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>20</v>
+      </c>
+      <c r="C4" s="3">
+        <v>45</v>
+      </c>
+      <c r="D4" s="3">
+        <v>30</v>
+      </c>
+      <c r="E4" s="3">
+        <v>5</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>20</v>
+      </c>
+      <c r="C5" s="3">
+        <v>45</v>
+      </c>
+      <c r="D5" s="3">
+        <v>30</v>
+      </c>
+      <c r="E5" s="3">
+        <v>5</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>20</v>
+      </c>
+      <c r="C6" s="3">
+        <v>30</v>
+      </c>
+      <c r="D6" s="3">
+        <v>40</v>
+      </c>
+      <c r="E6" s="3">
+        <v>10</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>20</v>
+      </c>
+      <c r="C7" s="3">
+        <v>30</v>
+      </c>
+      <c r="D7" s="3">
+        <v>40</v>
+      </c>
+      <c r="E7" s="3">
+        <v>10</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <f>SUM(B8:F8)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>15</v>
+      </c>
+      <c r="C8" s="3">
+        <v>20</v>
+      </c>
+      <c r="D8" s="3">
+        <v>50</v>
+      </c>
+      <c r="E8" s="3">
+        <v>10</v>
+      </c>
+      <c r="F8" s="3">
+        <v>5</v>
+      </c>
+      <c r="G8">
+        <f>SUM(B8:F8)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>10</v>
+      </c>
+      <c r="C9" s="3">
+        <v>30</v>
+      </c>
+      <c r="D9" s="3">
+        <v>35</v>
+      </c>
+      <c r="E9" s="3">
+        <v>10</v>
+      </c>
+      <c r="F9" s="3">
+        <v>15</v>
+      </c>
+      <c r="G9">
+        <f>SUM(B9:F9)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>5</v>
+      </c>
+      <c r="C10" s="3">
+        <v>10</v>
+      </c>
+      <c r="D10" s="3">
+        <v>35</v>
+      </c>
+      <c r="E10" s="3">
+        <v>20</v>
+      </c>
+      <c r="F10" s="3">
+        <v>30</v>
+      </c>
+      <c r="G10">
+        <f>SUM(B10:F10)</f>
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>